<commit_message>
some updates to match new thiazide concept set
</commit_message>
<xml_diff>
--- a/patient_addition/data.xlsx
+++ b/patient_addition/data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erc53/Github/iDiA_Rules/patient_addition/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erc53/Github/ddi-cds/patient_addition/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5272873-0A52-7143-B112-F6BFE4067B1D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12A78639-1040-3046-B86E-C35C07376A6D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4780" yWindow="-19680" windowWidth="28040" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -954,7 +954,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A527" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E551" sqref="E551"/>
+      <selection pane="bottomLeft" activeCell="D543" sqref="D543"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12410,7 +12410,7 @@
         <v>1574</v>
       </c>
       <c r="D543">
-        <v>974196</v>
+        <v>19019044</v>
       </c>
       <c r="E543" s="1">
         <v>39491</v>
@@ -12536,7 +12536,7 @@
         <v>1575</v>
       </c>
       <c r="D549">
-        <v>974196</v>
+        <v>19019044</v>
       </c>
       <c r="E549" s="1">
         <v>39491</v>

</xml_diff>

<commit_message>
modified the citalopram - QT prolongation rule to include Tisdale risk factors
</commit_message>
<xml_diff>
--- a/patient_addition/data.xlsx
+++ b/patient_addition/data.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1023" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1044" uniqueCount="26">
   <si>
     <t xml:space="preserve">INSERT_TYPE</t>
   </si>
@@ -177,7 +177,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -188,6 +188,10 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -211,12 +215,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N1048576"/>
+  <dimension ref="A1:N618"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A562" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A581" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A596" activeCellId="0" sqref="A596"/>
+      <selection pane="bottomLeft" activeCell="G610" activeCellId="0" sqref="G610"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.0078125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12806,7 +12810,303 @@
         <v>4171047</v>
       </c>
     </row>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="598" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A598" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B598" s="0" t="n">
+        <v>1582</v>
+      </c>
+      <c r="D598" s="3" t="n">
+        <v>3005456</v>
+      </c>
+      <c r="E598" s="2" t="n">
+        <v>39491</v>
+      </c>
+      <c r="G598" s="0" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="H598" s="0" t="n">
+        <v>9557</v>
+      </c>
+    </row>
+    <row r="599" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A599" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B599" s="0" t="n">
+        <v>1583</v>
+      </c>
+      <c r="C599" s="0" t="n">
+        <v>1950</v>
+      </c>
+      <c r="K599" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L599" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="600" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A600" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B600" s="0" t="n">
+        <v>1583</v>
+      </c>
+      <c r="D600" s="0" t="n">
+        <v>1398937</v>
+      </c>
+      <c r="E600" s="2" t="n">
+        <v>39491</v>
+      </c>
+      <c r="F600" s="2" t="n">
+        <v>39565</v>
+      </c>
+    </row>
+    <row r="601" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A601" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B601" s="0" t="n">
+        <v>1583</v>
+      </c>
+      <c r="D601" s="0" t="n">
+        <v>950370</v>
+      </c>
+      <c r="E601" s="2" t="n">
+        <v>39491</v>
+      </c>
+      <c r="F601" s="2" t="n">
+        <v>39565</v>
+      </c>
+    </row>
+    <row r="602" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A602" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B602" s="0" t="n">
+        <v>1583</v>
+      </c>
+      <c r="D602" s="0" t="n">
+        <v>797617</v>
+      </c>
+      <c r="E602" s="2" t="n">
+        <v>39491</v>
+      </c>
+      <c r="F602" s="2" t="n">
+        <v>39565</v>
+      </c>
+    </row>
+    <row r="603" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A603" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B603" s="0" t="n">
+        <v>1583</v>
+      </c>
+      <c r="D603" s="0" t="n">
+        <v>1354860</v>
+      </c>
+      <c r="E603" s="2" t="n">
+        <v>39491</v>
+      </c>
+      <c r="F603" s="2" t="n">
+        <v>39565</v>
+      </c>
+    </row>
+    <row r="604" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A604" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B604" s="0" t="n">
+        <v>1583</v>
+      </c>
+      <c r="E604" s="2" t="n">
+        <v>39491</v>
+      </c>
+      <c r="F604" s="2" t="n">
+        <v>39565</v>
+      </c>
+      <c r="H604" s="0" t="n">
+        <v>9201</v>
+      </c>
+    </row>
+    <row r="605" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A605" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B605" s="0" t="n">
+        <v>1583</v>
+      </c>
+      <c r="D605" s="0" t="n">
+        <v>40223506</v>
+      </c>
+      <c r="E605" s="2" t="n">
+        <v>39491</v>
+      </c>
+      <c r="F605" s="2" t="n">
+        <v>39565</v>
+      </c>
+      <c r="I605" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="J605" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="M605" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="N605" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="606" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A606" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B606" s="0" t="n">
+        <v>1583</v>
+      </c>
+      <c r="D606" s="0" t="n">
+        <v>43219718</v>
+      </c>
+      <c r="E606" s="2" t="n">
+        <v>39491</v>
+      </c>
+      <c r="F606" s="2" t="n">
+        <v>39565</v>
+      </c>
+      <c r="I606" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="J606" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="M606" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="N606" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="607" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A607" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B607" s="0" t="n">
+        <v>1583</v>
+      </c>
+      <c r="D607" s="0" t="n">
+        <v>797637</v>
+      </c>
+      <c r="E607" s="2" t="n">
+        <v>39491</v>
+      </c>
+      <c r="F607" s="2" t="n">
+        <v>39565</v>
+      </c>
+      <c r="I607" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="J607" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="M607" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="N607" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="608" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A608" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B608" s="0" t="n">
+        <v>1583</v>
+      </c>
+      <c r="D608" s="0" t="n">
+        <v>19022281</v>
+      </c>
+      <c r="E608" s="2" t="n">
+        <v>39491</v>
+      </c>
+      <c r="F608" s="2" t="n">
+        <v>39565</v>
+      </c>
+      <c r="G608" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="I608" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="J608" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="M608" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="N608" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="609" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A609" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B609" s="0" t="n">
+        <v>1582</v>
+      </c>
+      <c r="D609" s="3" t="n">
+        <v>3005456</v>
+      </c>
+      <c r="E609" s="2" t="n">
+        <v>39491</v>
+      </c>
+      <c r="G609" s="0" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="H609" s="0" t="n">
+        <v>9557</v>
+      </c>
+    </row>
+    <row r="610" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E610" s="2"/>
+      <c r="F610" s="2"/>
+    </row>
+    <row r="611" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E611" s="2"/>
+      <c r="F611" s="2"/>
+    </row>
+    <row r="612" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E612" s="2"/>
+      <c r="F612" s="2"/>
+    </row>
+    <row r="613" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E613" s="2"/>
+      <c r="F613" s="2"/>
+    </row>
+    <row r="614" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E614" s="2"/>
+      <c r="F614" s="2"/>
+    </row>
+    <row r="615" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E615" s="2"/>
+      <c r="F615" s="2"/>
+    </row>
+    <row r="616" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E616" s="2"/>
+      <c r="F616" s="2"/>
+    </row>
+    <row r="617" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E617" s="2"/>
+      <c r="F617" s="2"/>
+    </row>
+    <row r="618" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E618" s="2"/>
+      <c r="F618" s="2"/>
+    </row>
   </sheetData>
   <autoFilter ref="A1:M487"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Updating DDI CDS App with recommendations based upon group discussion
</commit_message>
<xml_diff>
--- a/patient_addition/data.xlsx
+++ b/patient_addition/data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maxsibilla/Documents/Dev/ddi-cds/patient_addition/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89F5A983-F212-C546-BF3A-D7FAB6229FE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F8ED79F-3E2C-A347-A424-62341CDB131F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -126,12 +126,6 @@
     <t>itraconazole</t>
   </si>
   <si>
-    <t>Chronic kidney disease, stage 2 (N18.2 ICD10)</t>
-  </si>
-  <si>
-    <t>Acute renal failure, unspecified (N17.9 ICD10)</t>
-  </si>
-  <si>
     <t>ritonavir 100 MG Oral Capsule</t>
   </si>
   <si>
@@ -151,6 +145,12 @@
   </si>
   <si>
     <t xml:space="preserve">Citalopram-QT Prolonging Agent </t>
+  </si>
+  <si>
+    <t>Acute renal failure, unspecified (N17.9 ICD10-CN)</t>
+  </si>
+  <si>
+    <t>Chronic kidney disease, stage 2 (N18.2 ICD10-CN)</t>
   </si>
 </sst>
 </file>
@@ -563,9 +563,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q700"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A666" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A698" sqref="A698"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A605" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P693" sqref="P693"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -20937,7 +20937,7 @@
       <c r="N685" s="3"/>
       <c r="O685" s="3"/>
       <c r="P685" s="10" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
     </row>
     <row r="686" spans="1:17" x14ac:dyDescent="0.2">
@@ -20949,7 +20949,7 @@
       </c>
       <c r="C686" s="3"/>
       <c r="D686" s="10">
-        <v>45553437</v>
+        <v>35209275</v>
       </c>
       <c r="E686" s="5">
         <v>44318</v>
@@ -20967,7 +20967,7 @@
       <c r="N686" s="3"/>
       <c r="O686" s="3"/>
       <c r="P686" s="10" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
     </row>
     <row r="687" spans="1:17" x14ac:dyDescent="0.2">
@@ -21135,7 +21135,7 @@
       </c>
       <c r="O691" s="3"/>
       <c r="P691" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="Q691" s="3"/>
     </row>
@@ -21166,7 +21166,7 @@
       <c r="N692" s="3"/>
       <c r="O692" s="3"/>
       <c r="P692" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="Q692" s="3"/>
     </row>
@@ -21178,8 +21178,8 @@
         <v>99996</v>
       </c>
       <c r="C693" s="3"/>
-      <c r="D693" s="2">
-        <v>45567829</v>
+      <c r="D693" s="10">
+        <v>1421642</v>
       </c>
       <c r="E693" s="5">
         <v>44318</v>
@@ -21197,7 +21197,7 @@
       <c r="N693" s="3"/>
       <c r="O693" s="3"/>
       <c r="P693" s="2" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="Q693" s="3"/>
     </row>
@@ -21209,8 +21209,8 @@
         <v>99996</v>
       </c>
       <c r="C694" s="3"/>
-      <c r="D694" s="2">
-        <v>45553437</v>
+      <c r="D694" s="10">
+        <v>35209275</v>
       </c>
       <c r="E694" s="5">
         <v>44318</v>
@@ -21227,8 +21227,8 @@
       <c r="M694" s="3"/>
       <c r="N694" s="3"/>
       <c r="O694" s="3"/>
-      <c r="P694" s="2" t="s">
-        <v>32</v>
+      <c r="P694" s="10" t="s">
+        <v>40</v>
       </c>
       <c r="Q694" s="3"/>
     </row>
@@ -21261,7 +21261,7 @@
         <v>8532</v>
       </c>
       <c r="P695" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="696" spans="1:17" x14ac:dyDescent="0.2">
@@ -21291,7 +21291,7 @@
       <c r="N696" s="3"/>
       <c r="O696" s="3"/>
       <c r="P696" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="697" spans="1:17" x14ac:dyDescent="0.2">
@@ -21321,7 +21321,7 @@
       <c r="N697" s="3"/>
       <c r="O697" s="3"/>
       <c r="P697" s="10" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="698" spans="1:17" x14ac:dyDescent="0.2">
@@ -21386,7 +21386,7 @@
       </c>
       <c r="O699" s="3"/>
       <c r="P699" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="700" spans="1:17" x14ac:dyDescent="0.2">
@@ -21424,7 +21424,7 @@
       </c>
       <c r="O700" s="3"/>
       <c r="P700" s="10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating tizanidine ddi-cds app to support new patient profiles
</commit_message>
<xml_diff>
--- a/patient_addition/data.xlsx
+++ b/patient_addition/data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maxsibilla/Documents/Dev/ddi-cds/patient_addition/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F8ED79F-3E2C-A347-A424-62341CDB131F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5BE5BB7-344C-F74C-93C4-D51C873B62AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1227" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1283" uniqueCount="51">
   <si>
     <t>INSERT_TYPE</t>
   </si>
@@ -151,6 +151,36 @@
   </si>
   <si>
     <t>Chronic kidney disease, stage 2 (N18.2 ICD10-CN)</t>
+  </si>
+  <si>
+    <t>tizanidine 2 MG Oral Tablet</t>
+  </si>
+  <si>
+    <t>Tizanidine</t>
+  </si>
+  <si>
+    <t>Ciprofloxacin 100 MG/ML Oral Suspension</t>
+  </si>
+  <si>
+    <t>Ciprofloxacin</t>
+  </si>
+  <si>
+    <t>zafirlukast 10 MG Oral Tablet</t>
+  </si>
+  <si>
+    <t>zafirlukast</t>
+  </si>
+  <si>
+    <t>Fluvoxamine Maleate 25 MG Oral Tablet</t>
+  </si>
+  <si>
+    <t>Fluvoxamine</t>
+  </si>
+  <si>
+    <t>Phenylpropanolamine Hydrochloride 50 MG Chewable Tablet</t>
+  </si>
+  <si>
+    <t>Phenylpropanolamine</t>
   </si>
 </sst>
 </file>
@@ -561,11 +591,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q700"/>
+  <dimension ref="A1:Q724"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A605" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P693" sqref="P693"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A699" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F713" sqref="F713"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -21427,6 +21457,774 @@
         <v>36</v>
       </c>
     </row>
+    <row r="701" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A701" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B701" s="2">
+        <v>100001</v>
+      </c>
+      <c r="C701" s="2">
+        <v>1960</v>
+      </c>
+      <c r="D701" s="3"/>
+      <c r="E701" s="3"/>
+      <c r="F701" s="3"/>
+      <c r="G701" s="3"/>
+      <c r="H701" s="3"/>
+      <c r="I701" s="3"/>
+      <c r="J701" s="3"/>
+      <c r="K701" s="2">
+        <v>1</v>
+      </c>
+      <c r="L701" s="2">
+        <v>1</v>
+      </c>
+      <c r="M701" s="3"/>
+      <c r="N701" s="3"/>
+      <c r="O701" s="2">
+        <v>8532</v>
+      </c>
+    </row>
+    <row r="702" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A702" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B702" s="2">
+        <v>100001</v>
+      </c>
+      <c r="C702" s="3"/>
+      <c r="D702" s="3"/>
+      <c r="E702" s="5">
+        <v>44317</v>
+      </c>
+      <c r="F702" s="5">
+        <v>44323</v>
+      </c>
+      <c r="G702" s="3"/>
+      <c r="H702" s="2">
+        <v>9201</v>
+      </c>
+      <c r="I702" s="3"/>
+      <c r="J702" s="3"/>
+      <c r="K702" s="3"/>
+      <c r="L702" s="3"/>
+      <c r="M702" s="3"/>
+      <c r="N702" s="3"/>
+      <c r="O702" s="3"/>
+    </row>
+    <row r="703" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A703" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B703" s="2">
+        <v>100001</v>
+      </c>
+      <c r="C703" s="3"/>
+      <c r="D703" s="10">
+        <v>778474</v>
+      </c>
+      <c r="E703" s="5">
+        <v>44318</v>
+      </c>
+      <c r="F703" s="5">
+        <v>44318</v>
+      </c>
+      <c r="G703" s="3"/>
+      <c r="H703" s="3"/>
+      <c r="I703" s="3"/>
+      <c r="J703" s="3"/>
+      <c r="K703" s="3"/>
+      <c r="L703" s="3"/>
+      <c r="M703" s="3"/>
+      <c r="N703" s="3"/>
+      <c r="O703" s="3"/>
+      <c r="P703" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="704" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A704" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B704" s="2">
+        <v>100001</v>
+      </c>
+      <c r="C704" s="3"/>
+      <c r="D704" s="10">
+        <v>778478</v>
+      </c>
+      <c r="E704" s="5">
+        <v>44319</v>
+      </c>
+      <c r="F704" s="5">
+        <v>44319</v>
+      </c>
+      <c r="G704" s="3"/>
+      <c r="H704" s="3"/>
+      <c r="I704" s="2">
+        <v>1</v>
+      </c>
+      <c r="J704" s="2">
+        <v>10</v>
+      </c>
+      <c r="K704" s="3"/>
+      <c r="L704" s="3"/>
+      <c r="M704" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="N704" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O704" s="3"/>
+      <c r="P704" s="10" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="705" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A705" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B705" s="2">
+        <v>100001</v>
+      </c>
+      <c r="C705" s="3"/>
+      <c r="D705" s="10">
+        <v>19075391</v>
+      </c>
+      <c r="E705" s="5">
+        <v>44319</v>
+      </c>
+      <c r="F705" s="5">
+        <v>44319</v>
+      </c>
+      <c r="G705" s="3"/>
+      <c r="H705" s="3"/>
+      <c r="I705" s="2">
+        <v>1</v>
+      </c>
+      <c r="J705" s="2">
+        <v>10</v>
+      </c>
+      <c r="K705" s="3"/>
+      <c r="L705" s="3"/>
+      <c r="M705" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="N705" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O705" s="3"/>
+      <c r="P705" s="10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="706" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A706" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B706" s="2">
+        <v>100001</v>
+      </c>
+      <c r="C706" s="3"/>
+      <c r="D706" s="10">
+        <v>1797513</v>
+      </c>
+      <c r="E706" s="5">
+        <v>44318</v>
+      </c>
+      <c r="F706" s="5">
+        <v>44318</v>
+      </c>
+      <c r="G706" s="3"/>
+      <c r="H706" s="3"/>
+      <c r="I706" s="3"/>
+      <c r="J706" s="3"/>
+      <c r="K706" s="3"/>
+      <c r="L706" s="3"/>
+      <c r="M706" s="3"/>
+      <c r="N706" s="3"/>
+      <c r="O706" s="3"/>
+      <c r="P706" s="10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="707" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A707" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B707" s="2">
+        <v>100002</v>
+      </c>
+      <c r="C707" s="2">
+        <v>1960</v>
+      </c>
+      <c r="D707" s="3"/>
+      <c r="E707" s="3"/>
+      <c r="F707" s="3"/>
+      <c r="G707" s="3"/>
+      <c r="H707" s="3"/>
+      <c r="I707" s="3"/>
+      <c r="J707" s="3"/>
+      <c r="K707" s="2">
+        <v>1</v>
+      </c>
+      <c r="L707" s="2">
+        <v>1</v>
+      </c>
+      <c r="M707" s="3"/>
+      <c r="N707" s="3"/>
+      <c r="O707" s="2">
+        <v>8532</v>
+      </c>
+    </row>
+    <row r="708" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A708" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B708" s="2">
+        <v>100002</v>
+      </c>
+      <c r="C708" s="3"/>
+      <c r="D708" s="3"/>
+      <c r="E708" s="5">
+        <v>44317</v>
+      </c>
+      <c r="F708" s="5">
+        <v>44323</v>
+      </c>
+      <c r="G708" s="3"/>
+      <c r="H708" s="2">
+        <v>9201</v>
+      </c>
+      <c r="I708" s="3"/>
+      <c r="J708" s="3"/>
+      <c r="K708" s="3"/>
+      <c r="L708" s="3"/>
+      <c r="M708" s="3"/>
+      <c r="N708" s="3"/>
+      <c r="O708" s="3"/>
+    </row>
+    <row r="709" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A709" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B709" s="2">
+        <v>100002</v>
+      </c>
+      <c r="C709" s="3"/>
+      <c r="D709" s="10">
+        <v>778474</v>
+      </c>
+      <c r="E709" s="5">
+        <v>44318</v>
+      </c>
+      <c r="F709" s="5">
+        <v>44318</v>
+      </c>
+      <c r="G709" s="3"/>
+      <c r="H709" s="3"/>
+      <c r="I709" s="3"/>
+      <c r="J709" s="3"/>
+      <c r="K709" s="3"/>
+      <c r="L709" s="3"/>
+      <c r="M709" s="3"/>
+      <c r="N709" s="3"/>
+      <c r="O709" s="3"/>
+      <c r="P709" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="710" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A710" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B710" s="2">
+        <v>100002</v>
+      </c>
+      <c r="C710" s="3"/>
+      <c r="D710" s="10">
+        <v>778478</v>
+      </c>
+      <c r="E710" s="5">
+        <v>44319</v>
+      </c>
+      <c r="F710" s="5">
+        <v>44319</v>
+      </c>
+      <c r="G710" s="3"/>
+      <c r="H710" s="3"/>
+      <c r="I710" s="2">
+        <v>1</v>
+      </c>
+      <c r="J710" s="2">
+        <v>10</v>
+      </c>
+      <c r="K710" s="3"/>
+      <c r="L710" s="3"/>
+      <c r="M710" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="N710" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O710" s="3"/>
+      <c r="P710" s="10" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="711" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A711" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B711" s="2">
+        <v>100002</v>
+      </c>
+      <c r="C711" s="3"/>
+      <c r="D711" s="10">
+        <v>1111710</v>
+      </c>
+      <c r="E711" s="5">
+        <v>44319</v>
+      </c>
+      <c r="F711" s="5">
+        <v>44319</v>
+      </c>
+      <c r="G711" s="3"/>
+      <c r="H711" s="3"/>
+      <c r="I711" s="2">
+        <v>1</v>
+      </c>
+      <c r="J711" s="2">
+        <v>10</v>
+      </c>
+      <c r="K711" s="3"/>
+      <c r="L711" s="3"/>
+      <c r="M711" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="N711" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O711" s="3"/>
+      <c r="P711" s="10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="712" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A712" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B712" s="2">
+        <v>100002</v>
+      </c>
+      <c r="C712" s="3"/>
+      <c r="D712" s="10">
+        <v>1111706</v>
+      </c>
+      <c r="E712" s="5">
+        <v>44318</v>
+      </c>
+      <c r="F712" s="5">
+        <v>44318</v>
+      </c>
+      <c r="G712" s="3"/>
+      <c r="H712" s="3"/>
+      <c r="I712" s="3"/>
+      <c r="J712" s="3"/>
+      <c r="K712" s="3"/>
+      <c r="L712" s="3"/>
+      <c r="M712" s="3"/>
+      <c r="N712" s="3"/>
+      <c r="O712" s="3"/>
+      <c r="P712" s="10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="713" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A713" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B713" s="2">
+        <v>100003</v>
+      </c>
+      <c r="C713" s="2">
+        <v>1960</v>
+      </c>
+      <c r="D713" s="3"/>
+      <c r="E713" s="3"/>
+      <c r="F713" s="3"/>
+      <c r="G713" s="3"/>
+      <c r="H713" s="3"/>
+      <c r="I713" s="3"/>
+      <c r="J713" s="3"/>
+      <c r="K713" s="2">
+        <v>1</v>
+      </c>
+      <c r="L713" s="2">
+        <v>1</v>
+      </c>
+      <c r="M713" s="3"/>
+      <c r="N713" s="3"/>
+      <c r="O713" s="2">
+        <v>8532</v>
+      </c>
+    </row>
+    <row r="714" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A714" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B714" s="2">
+        <v>100003</v>
+      </c>
+      <c r="C714" s="3"/>
+      <c r="D714" s="3"/>
+      <c r="E714" s="5">
+        <v>44317</v>
+      </c>
+      <c r="F714" s="5">
+        <v>44323</v>
+      </c>
+      <c r="G714" s="3"/>
+      <c r="H714" s="2">
+        <v>9201</v>
+      </c>
+      <c r="I714" s="3"/>
+      <c r="J714" s="3"/>
+      <c r="K714" s="3"/>
+      <c r="L714" s="3"/>
+      <c r="M714" s="3"/>
+      <c r="N714" s="3"/>
+      <c r="O714" s="3"/>
+    </row>
+    <row r="715" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A715" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B715" s="2">
+        <v>100003</v>
+      </c>
+      <c r="C715" s="3"/>
+      <c r="D715" s="10">
+        <v>778474</v>
+      </c>
+      <c r="E715" s="5">
+        <v>44318</v>
+      </c>
+      <c r="F715" s="5">
+        <v>44318</v>
+      </c>
+      <c r="G715" s="3"/>
+      <c r="H715" s="3"/>
+      <c r="I715" s="3"/>
+      <c r="J715" s="3"/>
+      <c r="K715" s="3"/>
+      <c r="L715" s="3"/>
+      <c r="M715" s="3"/>
+      <c r="N715" s="3"/>
+      <c r="O715" s="3"/>
+      <c r="P715" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="716" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A716" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B716" s="2">
+        <v>100003</v>
+      </c>
+      <c r="C716" s="3"/>
+      <c r="D716" s="10">
+        <v>778478</v>
+      </c>
+      <c r="E716" s="5">
+        <v>44319</v>
+      </c>
+      <c r="F716" s="5">
+        <v>44319</v>
+      </c>
+      <c r="G716" s="3"/>
+      <c r="H716" s="3"/>
+      <c r="I716" s="2">
+        <v>1</v>
+      </c>
+      <c r="J716" s="2">
+        <v>10</v>
+      </c>
+      <c r="K716" s="3"/>
+      <c r="L716" s="3"/>
+      <c r="M716" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="N716" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O716" s="3"/>
+      <c r="P716" s="10" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="717" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A717" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B717" s="2">
+        <v>100003</v>
+      </c>
+      <c r="C717" s="3"/>
+      <c r="D717" s="10">
+        <v>40174735</v>
+      </c>
+      <c r="E717" s="5">
+        <v>44319</v>
+      </c>
+      <c r="F717" s="5">
+        <v>44319</v>
+      </c>
+      <c r="G717" s="3"/>
+      <c r="H717" s="3"/>
+      <c r="I717" s="2">
+        <v>1</v>
+      </c>
+      <c r="J717" s="2">
+        <v>10</v>
+      </c>
+      <c r="K717" s="3"/>
+      <c r="L717" s="3"/>
+      <c r="M717" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="N717" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O717" s="3"/>
+      <c r="P717" s="10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="718" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A718" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B718" s="2">
+        <v>100003</v>
+      </c>
+      <c r="C718" s="3"/>
+      <c r="D718" s="10">
+        <v>751412</v>
+      </c>
+      <c r="E718" s="5">
+        <v>44318</v>
+      </c>
+      <c r="F718" s="5">
+        <v>44318</v>
+      </c>
+      <c r="G718" s="3"/>
+      <c r="H718" s="3"/>
+      <c r="I718" s="3"/>
+      <c r="J718" s="3"/>
+      <c r="K718" s="3"/>
+      <c r="L718" s="3"/>
+      <c r="M718" s="3"/>
+      <c r="N718" s="3"/>
+      <c r="O718" s="3"/>
+      <c r="P718" s="10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="719" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A719" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B719" s="2">
+        <v>100004</v>
+      </c>
+      <c r="C719" s="2">
+        <v>1960</v>
+      </c>
+      <c r="D719" s="3"/>
+      <c r="E719" s="3"/>
+      <c r="F719" s="3"/>
+      <c r="G719" s="3"/>
+      <c r="H719" s="3"/>
+      <c r="I719" s="3"/>
+      <c r="J719" s="3"/>
+      <c r="K719" s="2">
+        <v>1</v>
+      </c>
+      <c r="L719" s="2">
+        <v>1</v>
+      </c>
+      <c r="M719" s="3"/>
+      <c r="N719" s="3"/>
+      <c r="O719" s="2">
+        <v>8532</v>
+      </c>
+    </row>
+    <row r="720" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A720" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B720" s="2">
+        <v>100004</v>
+      </c>
+      <c r="C720" s="3"/>
+      <c r="D720" s="3"/>
+      <c r="E720" s="5">
+        <v>44317</v>
+      </c>
+      <c r="F720" s="5">
+        <v>44323</v>
+      </c>
+      <c r="G720" s="3"/>
+      <c r="H720" s="2">
+        <v>9201</v>
+      </c>
+      <c r="I720" s="3"/>
+      <c r="J720" s="3"/>
+      <c r="K720" s="3"/>
+      <c r="L720" s="3"/>
+      <c r="M720" s="3"/>
+      <c r="N720" s="3"/>
+      <c r="O720" s="3"/>
+    </row>
+    <row r="721" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A721" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B721" s="2">
+        <v>100004</v>
+      </c>
+      <c r="C721" s="3"/>
+      <c r="D721" s="10">
+        <v>778474</v>
+      </c>
+      <c r="E721" s="5">
+        <v>44318</v>
+      </c>
+      <c r="F721" s="5">
+        <v>44318</v>
+      </c>
+      <c r="G721" s="3"/>
+      <c r="H721" s="3"/>
+      <c r="I721" s="3"/>
+      <c r="J721" s="3"/>
+      <c r="K721" s="3"/>
+      <c r="L721" s="3"/>
+      <c r="M721" s="3"/>
+      <c r="N721" s="3"/>
+      <c r="O721" s="3"/>
+      <c r="P721" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="722" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A722" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B722" s="2">
+        <v>100004</v>
+      </c>
+      <c r="C722" s="3"/>
+      <c r="D722" s="10">
+        <v>778478</v>
+      </c>
+      <c r="E722" s="5">
+        <v>44319</v>
+      </c>
+      <c r="F722" s="5">
+        <v>44319</v>
+      </c>
+      <c r="G722" s="3"/>
+      <c r="H722" s="3"/>
+      <c r="I722" s="2">
+        <v>1</v>
+      </c>
+      <c r="J722" s="2">
+        <v>10</v>
+      </c>
+      <c r="K722" s="3"/>
+      <c r="L722" s="3"/>
+      <c r="M722" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="N722" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O722" s="3"/>
+      <c r="P722" s="10" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="723" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A723" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B723" s="2">
+        <v>100004</v>
+      </c>
+      <c r="C723" s="3"/>
+      <c r="D723" s="10">
+        <v>40243565</v>
+      </c>
+      <c r="E723" s="5">
+        <v>44319</v>
+      </c>
+      <c r="F723" s="5">
+        <v>44319</v>
+      </c>
+      <c r="G723" s="3"/>
+      <c r="H723" s="3"/>
+      <c r="I723" s="2">
+        <v>1</v>
+      </c>
+      <c r="J723" s="2">
+        <v>10</v>
+      </c>
+      <c r="K723" s="3"/>
+      <c r="L723" s="3"/>
+      <c r="M723" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="N723" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O723" s="3"/>
+      <c r="P723" s="10" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="724" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A724" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B724" s="2">
+        <v>100004</v>
+      </c>
+      <c r="C724" s="3"/>
+      <c r="D724" s="10">
+        <v>1139993</v>
+      </c>
+      <c r="E724" s="5">
+        <v>44318</v>
+      </c>
+      <c r="F724" s="5">
+        <v>44318</v>
+      </c>
+      <c r="G724" s="3"/>
+      <c r="H724" s="3"/>
+      <c r="I724" s="3"/>
+      <c r="J724" s="3"/>
+      <c r="K724" s="3"/>
+      <c r="L724" s="3"/>
+      <c r="M724" s="3"/>
+      <c r="N724" s="3"/>
+      <c r="O724" s="3"/>
+      <c r="P724" s="10" t="s">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:M487" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>